<commit_message>
fix authen flow, implement email sending
</commit_message>
<xml_diff>
--- a/Web/public/templates/users-import-template.xlsx
+++ b/Web/public/templates/users-import-template.xlsx
@@ -1,44 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\SkyTimeHub\Web\public\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B6BDF-AB20-4C8C-B4E3-F8E86C118049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>employeeId</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>departmentId</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>joinDate</t>
+  </si>
+  <si>
+    <t>EMP260001</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>2026-01-15</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>maikhaanh11205@gmail.com</t>
+  </si>
+  <si>
+    <t>Kha Em</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,17 +105,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,103 +451,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="30.796875" customWidth="1"/>
+    <col min="3" max="3" width="20.796875" customWidth="1"/>
+    <col min="4" max="4" width="18.796875" customWidth="1"/>
+    <col min="5" max="5" width="12.796875" customWidth="1"/>
+    <col min="6" max="6" width="25.796875" customWidth="1"/>
+    <col min="7" max="7" width="18.796875" customWidth="1"/>
+    <col min="8" max="8" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>employeeId</v>
-      </c>
-      <c r="B1" t="str">
-        <v>email</v>
-      </c>
-      <c r="C1" t="str">
-        <v>username</v>
-      </c>
-      <c r="D1" t="str">
-        <v>role</v>
-      </c>
-      <c r="E1" t="str">
-        <v>departmentId</v>
-      </c>
-      <c r="F1" t="str">
-        <v>position</v>
-      </c>
-      <c r="G1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="H1" t="str">
-        <v>joinDate</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>EMP260001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>john.doe@example.com</v>
-      </c>
-      <c r="C2" t="str">
-        <v>John Doe</v>
-      </c>
-      <c r="D2" t="str">
-        <v>employee</v>
-      </c>
-      <c r="E2" t="str">
-        <v>1</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Software Engineer</v>
-      </c>
-      <c r="G2" t="str">
-        <v>+84 123 456 789</v>
-      </c>
-      <c r="H2" t="str">
-        <v>2026-01-15</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v/>
-      </c>
-      <c r="B3" t="str">
-        <v>jane.smith@example.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Jane Smith</v>
-      </c>
-      <c r="D3" t="str">
-        <v>hr</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2</v>
-      </c>
-      <c r="F3" t="str">
-        <v>HR Manager</v>
-      </c>
-      <c r="G3" t="str">
-        <v>+84 987 654 321</v>
-      </c>
-      <c r="H3" t="str">
-        <v>2026-02-01</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D64BDD2D-7AF1-4B49-81C4-46E20F2BE80C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError sqref="A1:F1 A3 A2 D2:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add column gender, fix bug cc update leave_request
</commit_message>
<xml_diff>
--- a/Web/public/templates/users-import-template.xlsx
+++ b/Web/public/templates/users-import-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\SkyTimeHub\Web\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B6BDF-AB20-4C8C-B4E3-F8E86C118049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6BEC37-C2C5-4E28-BB25-BEB2DFDE8E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>employeeId</t>
   </si>
@@ -43,9 +43,6 @@
     <t>joinDate</t>
   </si>
   <si>
-    <t>EMP260001</t>
-  </si>
-  <si>
     <t>employee</t>
   </si>
   <si>
@@ -61,10 +58,19 @@
     <t/>
   </si>
   <si>
+    <t>Kha Em</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>MAI122</t>
+  </si>
+  <si>
     <t>maikhaanh11205@gmail.com</t>
-  </si>
-  <si>
-    <t>Kha Em</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -470,7 +476,7 @@
     <col min="8" max="8" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,33 +498,39 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +539,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A3 A2 D2:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A3 D2:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add user required fields, resend activation link button
</commit_message>
<xml_diff>
--- a/Web/public/templates/users-import-template.xlsx
+++ b/Web/public/templates/users-import-template.xlsx
@@ -1,94 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\SkyTimeHub\Web\public\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6BEC37-C2C5-4E28-BB25-BEB2DFDE8E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>employeeId</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>departmentId</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>joinDate</t>
-  </si>
-  <si>
-    <t>employee</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>2026-01-15</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Kha Em</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>MAI122</t>
-  </si>
-  <si>
-    <t>maikhaanh11205@gmail.com</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,28 +61,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -457,89 +396,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="2" max="2" width="30.796875" customWidth="1"/>
-    <col min="3" max="3" width="20.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.796875" customWidth="1"/>
-    <col min="5" max="5" width="12.796875" customWidth="1"/>
-    <col min="6" max="6" width="25.796875" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>employeeId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>email</v>
+      </c>
+      <c r="C1" t="str">
+        <v>username</v>
+      </c>
+      <c r="D1" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="E1" t="str">
+        <v>gender</v>
+      </c>
+      <c r="F1" t="str">
+        <v>dateOfBirth</v>
+      </c>
+      <c r="G1" t="str">
+        <v>address</v>
+      </c>
+      <c r="H1" t="str">
+        <v>role</v>
+      </c>
+      <c r="I1" t="str">
+        <v>departmentId</v>
+      </c>
+      <c r="J1" t="str">
+        <v>position</v>
+      </c>
+      <c r="K1" t="str">
+        <v>joinDate</v>
+      </c>
+      <c r="L1" t="str">
+        <v>officialContractDate</v>
+      </c>
+      <c r="M1" t="str">
+        <v>contractType</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>EMP240001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>john@example.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="D2" t="str">
+        <v>0901234567</v>
+      </c>
+      <c r="E2" t="str">
+        <v>male</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1995-06-15</v>
+      </c>
+      <c r="G2" t="str">
+        <v>123 Main St, Hanoi</v>
+      </c>
+      <c r="H2" t="str">
+        <v>employee</v>
+      </c>
+      <c r="I2" t="str">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J2" t="str">
+        <v>Software Engineer</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2024-01-15</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2024-03-15</v>
+      </c>
+      <c r="M2" t="str">
+        <v>full_time</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>EMP240002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>jane@example.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Jane Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>0912345678</v>
+      </c>
+      <c r="E3" t="str">
+        <v>female</v>
+      </c>
+      <c r="F3" t="str">
+        <v>1998-03-20</v>
+      </c>
+      <c r="G3" t="str">
+        <v>456 Le Loi, HCM</v>
+      </c>
+      <c r="H3" t="str">
+        <v>hr</v>
+      </c>
+      <c r="I3" t="str">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
+      <c r="J3" t="str">
+        <v>HR Manager</v>
+      </c>
+      <c r="K3" t="str">
+        <v>2024-02-01</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2024-02-01</v>
+      </c>
+      <c r="M3" t="str">
+        <v>probation</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D64BDD2D-7AF1-4B49-81C4-46E20F2BE80C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 A3 D2:F2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>